<commit_message>
added sprint 3 standup
</commit_message>
<xml_diff>
--- a/docs/Sprint 3/Copy of Copy of Burn Down.xlsx
+++ b/docs/Sprint 3/Copy of Copy of Burn Down.xlsx
@@ -164,11 +164,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="825206880"/>
-        <c:axId val="596884456"/>
+        <c:axId val="1070518669"/>
+        <c:axId val="1089155213"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="825206880"/>
+        <c:axId val="1070518669"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -210,10 +210,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="596884456"/>
+        <c:crossAx val="1089155213"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="596884456"/>
+        <c:axId val="1089155213"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -284,7 +284,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="825206880"/>
+        <c:crossAx val="1070518669"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -576,13 +576,19 @@
       <c r="B3" s="3">
         <v>12.0</v>
       </c>
+      <c r="C3" s="3">
+        <v>16.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="5">
-        <v>43785.0</v>
+        <v>43787.0</v>
       </c>
       <c r="B4" s="3">
         <v>8.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>6.0</v>
       </c>
     </row>
     <row r="5">

</xml_diff>